<commit_message>
Anexo de leyenda a documentos
</commit_message>
<xml_diff>
--- a/A-DOCUMENTACION/010. CASOS DE PRUEBA.xlsx
+++ b/A-DOCUMENTACION/010. CASOS DE PRUEBA.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SISTEMAS\Documents\GitHub\Proyectos\A-DOCUMENTACION\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SISTEMAS\Documents\CLAUDIA\PROYECTOS\DOCUMENTACION\A-PROYECTOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9180" windowHeight="7380"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9180" windowHeight="7380" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
   <si>
     <r>
       <t xml:space="preserve">Revisión. </t>
@@ -172,6 +172,9 @@
   </si>
   <si>
     <t xml:space="preserve">Código. </t>
+  </si>
+  <si>
+    <t>Se prohíbe la reproducción parcial o total de este documento, por cualquier medio, sin autorización de la Dirección de Comercial de Carnes Frías del Norte. Este documento contiene información confidencial y de uso exclusivo de personal de CCFN.</t>
   </si>
 </sst>
 </file>
@@ -342,7 +345,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -441,8 +444,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -912,8 +918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1007,11 +1013,11 @@
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="18"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="38"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="18" t="s">
@@ -1019,11 +1025,11 @@
       </c>
       <c r="C10" s="18"/>
       <c r="D10" s="18"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="18" t="s">
@@ -1031,11 +1037,11 @@
       </c>
       <c r="C11" s="18"/>
       <c r="D11" s="18"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="38"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="18" t="s">
@@ -1043,11 +1049,11 @@
       </c>
       <c r="C12" s="18"/>
       <c r="D12" s="18"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="18" t="s">
@@ -1127,10 +1133,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:T26"/>
+  <dimension ref="B2:T31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:I2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1566,8 +1572,50 @@
       <c r="I26" s="19"/>
       <c r="J26" s="19"/>
     </row>
+    <row r="29" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B29" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
+      <c r="K29" s="39"/>
+      <c r="L29" s="39"/>
+      <c r="M29" s="39"/>
+      <c r="N29" s="39"/>
+      <c r="O29" s="39"/>
+      <c r="P29" s="39"/>
+      <c r="Q29" s="39"/>
+      <c r="R29" s="39"/>
+      <c r="S29" s="39"/>
+      <c r="T29" s="39"/>
+    </row>
+    <row r="30" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
+    </row>
+    <row r="31" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="D31" s="38"/>
+      <c r="E31" s="38"/>
+      <c r="F31" s="38"/>
+      <c r="G31" s="38"/>
+      <c r="H31" s="38"/>
+      <c r="I31" s="38"/>
+      <c r="J31" s="38"/>
+    </row>
   </sheetData>
-  <mergeCells count="66">
+  <mergeCells count="67">
+    <mergeCell ref="B29:T29"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="J2:J4"/>

</xml_diff>